<commit_message>
Implemented writer to excel and fix known issue in 3.2
</commit_message>
<xml_diff>
--- a/ocelot/data/format.xlsx
+++ b/ocelot/data/format.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="135">
   <si>
     <t>parent</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>property name</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
@@ -760,7 +763,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -796,7 +799,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -819,7 +822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -839,7 +842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -859,7 +862,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -882,7 +885,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -899,7 +902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -916,7 +919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -936,7 +939,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -956,7 +959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -979,7 +982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -999,7 +1002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -1059,7 +1062,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>100</v>
       </c>
@@ -1414,7 +1417,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>104</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -1454,7 +1457,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -1494,7 +1497,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -1511,7 +1514,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>104</v>
       </c>
@@ -1522,7 +1525,7 @@
         <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F37" t="s">
         <v>111</v>
@@ -1830,7 +1833,7 @@
         <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="C53" t="s">
         <v>51</v>
@@ -2032,7 +2035,7 @@
   <autoFilter ref="A1:G62">
     <filterColumn colId="0">
       <filters>
-        <filter val="dataset"/>
+        <filter val="parameters"/>
       </filters>
     </filterColumn>
     <sortState ref="A2:G62">

</xml_diff>

<commit_message>
worked on combined production.  Not fully tested yet.
</commit_message>
<xml_diff>
--- a/ocelot/data/format.xlsx
+++ b/ocelot/data/format.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="137">
   <si>
     <t>parent</t>
   </si>
@@ -92,9 +92,6 @@
     <t>100: activityName</t>
   </si>
   <si>
-    <t>in dataframe</t>
-  </si>
-  <si>
     <t>activity name</t>
   </si>
   <si>
@@ -432,6 +429,15 @@
   </si>
   <si>
     <t>mean</t>
+  </si>
+  <si>
+    <t>standard deviation 95%</t>
+  </si>
+  <si>
+    <t>standardDeviation95</t>
+  </si>
+  <si>
+    <t>in data frame</t>
   </si>
 </sst>
 </file>
@@ -758,11 +764,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -795,12 +802,12 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -809,21 +816,21 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -832,7 +839,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -841,13 +848,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
         <v>100</v>
       </c>
-      <c r="B4" t="s">
-        <v>101</v>
-      </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -855,38 +862,38 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -895,15 +902,15 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -918,9 +925,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -932,15 +939,15 @@
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -949,7 +956,7 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
@@ -958,9 +965,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -969,21 +976,21 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -992,7 +999,7 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
         <v>19</v>
@@ -1001,9 +1008,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -1018,52 +1025,52 @@
         <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1072,21 +1079,21 @@
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -1095,108 +1102,108 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
         <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1207,24 +1214,24 @@
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
         <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -1233,13 +1240,13 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1253,35 +1260,35 @@
         <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -1290,56 +1297,56 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" t="s">
         <v>18</v>
       </c>
       <c r="F27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1350,38 +1357,38 @@
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E28" t="s">
         <v>18</v>
       </c>
       <c r="G28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29" t="s">
         <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" t="s">
         <v>16</v>
@@ -1390,18 +1397,18 @@
         <v>18</v>
       </c>
       <c r="F30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
         <v>16</v>
@@ -1410,35 +1417,35 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E32" t="s">
         <v>18</v>
       </c>
       <c r="F32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s">
         <v>4</v>
@@ -1450,18 +1457,18 @@
         <v>18</v>
       </c>
       <c r="F33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
@@ -1470,15 +1477,15 @@
         <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
@@ -1490,149 +1497,149 @@
         <v>18</v>
       </c>
       <c r="F35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
+        <v>110</v>
+      </c>
+      <c r="G37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
+        <v>72</v>
+      </c>
+      <c r="G38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" t="s">
+        <v>74</v>
+      </c>
+      <c r="G39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" t="s">
+        <v>73</v>
+      </c>
+      <c r="G41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>49</v>
       </c>
-      <c r="C36" t="s">
-        <v>52</v>
-      </c>
-      <c r="E36" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>104</v>
-      </c>
-      <c r="B37" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" t="s">
-        <v>111</v>
-      </c>
-      <c r="G37" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E38" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" t="s">
-        <v>73</v>
-      </c>
-      <c r="G38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" t="s">
-        <v>75</v>
-      </c>
-      <c r="G39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>49</v>
-      </c>
-      <c r="C40" t="s">
-        <v>52</v>
-      </c>
-      <c r="E40" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" t="s">
-        <v>74</v>
-      </c>
-      <c r="G41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" t="s">
-        <v>51</v>
-      </c>
-      <c r="E42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" t="s">
-        <v>94</v>
-      </c>
-      <c r="G42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>50</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
@@ -1644,18 +1651,18 @@
         <v>18</v>
       </c>
       <c r="F43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G43" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
         <v>16</v>
@@ -1664,15 +1671,15 @@
         <v>19</v>
       </c>
       <c r="F44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
@@ -1684,35 +1691,35 @@
         <v>18</v>
       </c>
       <c r="F45" t="s">
+        <v>131</v>
+      </c>
+      <c r="G45" t="s">
         <v>132</v>
       </c>
-      <c r="G45" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>49</v>
       </c>
-      <c r="C46" t="s">
-        <v>52</v>
-      </c>
-      <c r="E46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>50</v>
-      </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C47" t="s">
         <v>16</v>
@@ -1721,18 +1728,18 @@
         <v>18</v>
       </c>
       <c r="F47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G47" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
         <v>16</v>
@@ -1741,235 +1748,235 @@
         <v>19</v>
       </c>
       <c r="F48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E49" t="s">
         <v>18</v>
       </c>
       <c r="F49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E50" t="s">
         <v>18</v>
       </c>
       <c r="F50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E51" t="s">
         <v>18</v>
       </c>
       <c r="F51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52" t="s">
         <v>19</v>
       </c>
       <c r="F52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E53" t="s">
         <v>19</v>
       </c>
       <c r="F53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E54" t="s">
         <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E55" t="s">
         <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E56" t="s">
         <v>19</v>
       </c>
       <c r="F56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E57" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" t="s">
+        <v>119</v>
+      </c>
+      <c r="G57" t="s">
         <v>105</v>
-      </c>
-      <c r="E57" t="s">
-        <v>18</v>
-      </c>
-      <c r="F57" t="s">
-        <v>120</v>
-      </c>
-      <c r="G57" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E58" t="s">
         <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E59" t="s">
         <v>18</v>
       </c>
       <c r="F59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G59" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -1978,60 +1985,85 @@
         <v>16</v>
       </c>
       <c r="D60" t="s">
+        <v>85</v>
+      </c>
+      <c r="E60" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" t="s">
         <v>86</v>
       </c>
-      <c r="E60" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" t="s">
-        <v>87</v>
-      </c>
       <c r="G60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E61" t="s">
         <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C62" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E62" t="s">
         <v>19</v>
       </c>
       <c r="F62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G62" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" t="s">
+        <v>134</v>
+      </c>
+      <c r="C63" t="s">
+        <v>50</v>
+      </c>
+      <c r="E63" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" t="s">
+        <v>135</v>
+      </c>
+      <c r="G63" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G62">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="uncertainty"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:G62">
       <sortCondition ref="A1:A62"/>
     </sortState>

</xml_diff>

<commit_message>
validated every dataset against ifu.  yay!
</commit_message>
<xml_diff>
--- a/ocelot/data/format.xlsx
+++ b/ocelot/data/format.xlsx
@@ -68,9 +68,6 @@
     <t>allocation method</t>
   </si>
   <si>
-    <t>main reference product</t>
-  </si>
-  <si>
     <t>last operation</t>
   </si>
   <si>
@@ -444,6 +441,9 @@
   </si>
   <si>
     <t>name of transformations as keys, time of execution as elements</t>
+  </si>
+  <si>
+    <t>reference product</t>
   </si>
 </sst>
 </file>
@@ -775,7 +775,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,7 +793,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -802,33 +802,33 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -836,19 +836,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -856,76 +856,76 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
         <v>98</v>
       </c>
-      <c r="B4" t="s">
-        <v>99</v>
-      </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -933,62 +933,62 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
@@ -996,102 +996,102 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
         <v>20</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
@@ -1099,25 +1099,25 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1125,22 +1125,22 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1148,19 +1148,19 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1168,22 +1168,22 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1191,22 +1191,22 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1217,19 +1217,19 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1237,19 +1237,19 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1260,16 +1260,16 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1277,16 +1277,16 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1294,16 +1294,16 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1311,22 +1311,22 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1334,22 +1334,22 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1360,16 +1360,16 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1377,16 +1377,16 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1394,19 +1394,19 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -1414,670 +1414,670 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="s">
         <v>49</v>
       </c>
-      <c r="B42" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" t="s">
-        <v>50</v>
-      </c>
       <c r="E42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G45" t="s">
         <v>130</v>
-      </c>
-      <c r="G45" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F55" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C57" t="s">
+        <v>102</v>
+      </c>
+      <c r="E57" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" t="s">
+        <v>117</v>
+      </c>
+      <c r="G57" t="s">
         <v>103</v>
-      </c>
-      <c r="E57" t="s">
-        <v>18</v>
-      </c>
-      <c r="F57" t="s">
-        <v>118</v>
-      </c>
-      <c r="G57" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C59" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F59" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G59" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
       </c>
       <c r="C60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D60" t="s">
+        <v>83</v>
+      </c>
+      <c r="E60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" t="s">
         <v>84</v>
       </c>
-      <c r="E60" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" t="s">
-        <v>85</v>
-      </c>
       <c r="G60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C62" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E62" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B63" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E63" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63" t="s">
         <v>133</v>
       </c>
-      <c r="C63" t="s">
-        <v>50</v>
-      </c>
-      <c r="E63" t="s">
-        <v>19</v>
-      </c>
-      <c r="F63" t="s">
-        <v>134</v>
-      </c>
       <c r="G63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B64" t="s">
+        <v>136</v>
+      </c>
+      <c r="C64" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" t="s">
         <v>137</v>
       </c>
-      <c r="C64" t="s">
-        <v>51</v>
-      </c>
-      <c r="D64" t="s">
-        <v>138</v>
-      </c>
       <c r="E64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validator of datasets, independent of the source
also changed:
-unit is now mandatory in parameters
-pedigree is [5, 5, 5, 5, 5] if absent if uncertainty type is lognormal
or normal
-wrote utils.sel_data_frame(), but only useful on small dataframes, not
sure this is very helpful, I ended up not using it.
</commit_message>
<xml_diff>
--- a/ocelot/data/format.xlsx
+++ b/ocelot/data/format.xlsx
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="142">
   <si>
     <t>parent</t>
   </si>
   <si>
-    <t>format</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
     <t>XML tag name of the exchange</t>
   </si>
   <si>
-    <t>from list: ['from technosphere', 'from environment', 'reference product', 'byproduct', 'to environment']</t>
-  </si>
-  <si>
     <t>1035: unitName</t>
   </si>
   <si>
@@ -218,9 +212,6 @@
     <t>only for tag 'intermediateExchange'</t>
   </si>
   <si>
-    <t>from list: ['intermediateExchange', 'elementaryExchange']</t>
-  </si>
-  <si>
     <t>exchange type</t>
   </si>
   <si>
@@ -251,18 +242,12 @@
     <t>mu</t>
   </si>
   <si>
-    <t>sigma</t>
-  </si>
-  <si>
     <t>minimum</t>
   </si>
   <si>
     <t>maximum</t>
   </si>
   <si>
-    <t>from list: ['normal', 'lognormal', 'triangular', 'uniform', 'undefined']</t>
-  </si>
-  <si>
     <t>XML tag name of the first element after the uncertainty element</t>
   </si>
   <si>
@@ -425,9 +410,6 @@
     <t>public, licensees, results only, restricted</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>in dataset</t>
   </si>
   <si>
@@ -438,6 +420,39 @@
   </si>
   <si>
     <t>1712: unitName</t>
+  </si>
+  <si>
+    <t>intermediateExchange, elementaryExchange</t>
+  </si>
+  <si>
+    <t>from technosphere, from environment, reference product, byproduct, to environment</t>
+  </si>
+  <si>
+    <t>air, water, soil, natural resource</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>normal, lognormal, triangular, uniform, undefined</t>
+  </si>
+  <si>
+    <t>mandatory for lognormal and normal</t>
+  </si>
+  <si>
+    <t>mandatory for triangular, beta, uniform and undefined</t>
+  </si>
+  <si>
+    <t>mandatory for triangular, beta, gamma, uniform and undefined</t>
+  </si>
+  <si>
+    <t>mandatory for triangular</t>
+  </si>
+  <si>
+    <t>mandatory for lognormal</t>
+  </si>
+  <si>
+    <t>mandatory for undefined</t>
   </si>
 </sst>
 </file>
@@ -766,11 +781,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G65" sqref="G65"/>
+      <selection pane="bottomLeft" activeCell="F48" sqref="F48:F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,1308 +804,1342 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>132</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
         <v>18</v>
-      </c>
-      <c r="H11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H20" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H21" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" t="s">
-        <v>59</v>
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>131</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H22" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
       <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" t="s">
-        <v>58</v>
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>132</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H23" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>59</v>
       </c>
       <c r="F25" t="s">
         <v>16</v>
       </c>
       <c r="G25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H25" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>133</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F27" t="s">
         <v>16</v>
       </c>
       <c r="G27" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H27" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
         <v>16</v>
       </c>
+      <c r="G28" t="s">
+        <v>47</v>
+      </c>
       <c r="H28" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>57</v>
       </c>
       <c r="F29" t="s">
         <v>16</v>
       </c>
       <c r="G29" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H29" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" t="s">
+        <v>101</v>
+      </c>
+      <c r="H32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
         <v>32</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" t="s">
+        <v>98</v>
+      </c>
+      <c r="H33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" t="s">
+        <v>113</v>
+      </c>
+      <c r="H34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" t="s">
         <v>44</v>
       </c>
-      <c r="F31" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" t="s">
-        <v>101</v>
-      </c>
-      <c r="H31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" t="s">
-        <v>106</v>
-      </c>
-      <c r="H32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="F35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="s">
         <v>33</v>
       </c>
-      <c r="C33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" t="s">
-        <v>103</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" t="s">
-        <v>118</v>
-      </c>
-      <c r="H34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" t="s">
-        <v>102</v>
-      </c>
-      <c r="H36" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G39" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G40" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" t="s">
         <v>43</v>
       </c>
-      <c r="B41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" t="s">
-        <v>44</v>
-      </c>
       <c r="F41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G42" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H42" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G43" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G44" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G45" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G46" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" t="s">
+        <v>83</v>
+      </c>
+      <c r="H47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" t="s">
+        <v>105</v>
+      </c>
+      <c r="H48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" t="s">
+        <v>91</v>
+      </c>
+      <c r="D49" t="s">
+        <v>134</v>
+      </c>
+      <c r="E49" t="s">
+        <v>136</v>
+      </c>
+      <c r="F49" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" t="s">
+        <v>106</v>
+      </c>
+      <c r="H49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" t="s">
+        <v>107</v>
+      </c>
+      <c r="H50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" t="s">
+        <v>134</v>
+      </c>
+      <c r="E51" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" t="s">
+        <v>108</v>
+      </c>
+      <c r="H51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D52" t="s">
+        <v>134</v>
+      </c>
+      <c r="E52" t="s">
+        <v>136</v>
+      </c>
+      <c r="F52" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" t="s">
+        <v>109</v>
+      </c>
+      <c r="H52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" t="s">
         <v>43</v>
       </c>
-      <c r="B47" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" t="s">
-        <v>17</v>
-      </c>
-      <c r="G47" t="s">
-        <v>88</v>
-      </c>
-      <c r="H47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" t="s">
-        <v>96</v>
-      </c>
-      <c r="F48" t="s">
-        <v>16</v>
-      </c>
-      <c r="G48" t="s">
-        <v>110</v>
-      </c>
-      <c r="H48" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" t="s">
-        <v>96</v>
-      </c>
-      <c r="F49" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" t="s">
-        <v>111</v>
-      </c>
-      <c r="H49" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" t="s">
-        <v>115</v>
-      </c>
-      <c r="C50" t="s">
-        <v>96</v>
-      </c>
-      <c r="F50" t="s">
-        <v>16</v>
-      </c>
-      <c r="G50" t="s">
-        <v>112</v>
-      </c>
-      <c r="H50" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51" t="s">
-        <v>116</v>
-      </c>
-      <c r="C51" t="s">
-        <v>96</v>
-      </c>
-      <c r="F51" t="s">
-        <v>16</v>
-      </c>
-      <c r="G51" t="s">
-        <v>113</v>
-      </c>
-      <c r="H51" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="E53" t="s">
+        <v>137</v>
+      </c>
+      <c r="F53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" t="s">
+        <v>77</v>
+      </c>
+      <c r="H53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" t="s">
         <v>117</v>
       </c>
-      <c r="C52" t="s">
-        <v>96</v>
-      </c>
-      <c r="F52" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" t="s">
-        <v>114</v>
-      </c>
-      <c r="H52" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>42</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="C54" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54" t="s">
+        <v>136</v>
+      </c>
+      <c r="F54" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" t="s">
+        <v>74</v>
+      </c>
+      <c r="H54" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" t="s">
+        <v>43</v>
+      </c>
+      <c r="E55" t="s">
+        <v>138</v>
+      </c>
+      <c r="F55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" t="s">
         <v>76</v>
       </c>
-      <c r="C53" t="s">
-        <v>44</v>
-      </c>
-      <c r="F53" t="s">
-        <v>17</v>
-      </c>
-      <c r="G53" t="s">
-        <v>82</v>
-      </c>
-      <c r="H53" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>42</v>
-      </c>
-      <c r="B54" t="s">
-        <v>122</v>
-      </c>
-      <c r="C54" t="s">
-        <v>44</v>
-      </c>
-      <c r="F54" t="s">
-        <v>17</v>
-      </c>
-      <c r="G54" t="s">
-        <v>79</v>
-      </c>
-      <c r="H54" t="s">
+      <c r="H55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" t="s">
+        <v>43</v>
+      </c>
+      <c r="E56" t="s">
+        <v>139</v>
+      </c>
+      <c r="F56" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" t="s">
+        <v>78</v>
+      </c>
+      <c r="H56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="C57" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57" t="s">
+        <v>140</v>
+      </c>
+      <c r="F57" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" t="s">
+        <v>70</v>
+      </c>
+      <c r="H57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58" t="s">
+        <v>141</v>
+      </c>
+      <c r="F58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" t="s">
+        <v>119</v>
+      </c>
+      <c r="H58" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59" t="s">
+        <v>136</v>
+      </c>
+      <c r="F59" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" t="s">
+        <v>68</v>
+      </c>
+      <c r="H59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" t="s">
+        <v>43</v>
+      </c>
+      <c r="E60" t="s">
+        <v>136</v>
+      </c>
+      <c r="F60" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" t="s">
         <v>75</v>
       </c>
-      <c r="C55" t="s">
-        <v>44</v>
-      </c>
-      <c r="F55" t="s">
-        <v>17</v>
-      </c>
-      <c r="G55" t="s">
-        <v>81</v>
-      </c>
-      <c r="H55" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>42</v>
-      </c>
-      <c r="B56" t="s">
-        <v>126</v>
-      </c>
-      <c r="C56" t="s">
-        <v>44</v>
-      </c>
-      <c r="F56" t="s">
-        <v>17</v>
-      </c>
-      <c r="G56" t="s">
-        <v>83</v>
-      </c>
-      <c r="H56" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>42</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="H60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" t="s">
+        <v>135</v>
+      </c>
+      <c r="F61" t="s">
+        <v>15</v>
+      </c>
+      <c r="G61" t="s">
         <v>73</v>
       </c>
-      <c r="C57" t="s">
-        <v>44</v>
-      </c>
-      <c r="F57" t="s">
-        <v>17</v>
-      </c>
-      <c r="G57" t="s">
-        <v>73</v>
-      </c>
-      <c r="H57" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" t="s">
-        <v>74</v>
-      </c>
-      <c r="C58" t="s">
-        <v>44</v>
-      </c>
-      <c r="F58" t="s">
-        <v>17</v>
-      </c>
-      <c r="G58" t="s">
-        <v>74</v>
-      </c>
-      <c r="H58" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>42</v>
-      </c>
-      <c r="B59" t="s">
-        <v>123</v>
-      </c>
-      <c r="C59" t="s">
-        <v>44</v>
-      </c>
-      <c r="F59" t="s">
-        <v>17</v>
-      </c>
-      <c r="G59" t="s">
-        <v>124</v>
-      </c>
-      <c r="H59" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>42</v>
-      </c>
-      <c r="B60" t="s">
-        <v>71</v>
-      </c>
-      <c r="C60" t="s">
-        <v>44</v>
-      </c>
-      <c r="F60" t="s">
-        <v>17</v>
-      </c>
-      <c r="G60" t="s">
-        <v>71</v>
-      </c>
-      <c r="H60" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>42</v>
-      </c>
-      <c r="B61" t="s">
-        <v>72</v>
-      </c>
-      <c r="C61" t="s">
-        <v>44</v>
-      </c>
-      <c r="F61" t="s">
-        <v>17</v>
-      </c>
-      <c r="G61" t="s">
-        <v>80</v>
-      </c>
       <c r="H61" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="C62" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="E62" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="F62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G62" t="s">
-        <v>78</v>
-      </c>
-      <c r="H62" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>40</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
-      </c>
-      <c r="E63" t="s">
-        <v>128</v>
+        <v>13</v>
       </c>
       <c r="F63" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>95</v>
-      </c>
-      <c r="B64" t="s">
-        <v>41</v>
-      </c>
-      <c r="C64" t="s">
-        <v>14</v>
-      </c>
-      <c r="F64" t="s">
-        <v>16</v>
-      </c>
-      <c r="G64" t="s">
-        <v>136</v>
-      </c>
-      <c r="H64" t="s">
-        <v>41</v>
+        <v>15</v>
+      </c>
+      <c r="G63" t="s">
+        <v>130</v>
+      </c>
+      <c r="H63" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H63">
     <filterColumn colId="0">
       <filters>
-        <filter val="parameters"/>
+        <filter val="uncertainty"/>
       </filters>
     </filterColumn>
-    <sortState ref="A49:H63">
-      <sortCondition ref="G1:G64"/>
+    <sortState ref="A20:H30">
+      <sortCondition ref="F1:F64"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Placed "dataset_from_excel" and "dataset_to_excel" functions in "excel_utils.py"
</commit_message>
<xml_diff>
--- a/ocelot/data/format.xlsx
+++ b/ocelot/data/format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ocelot\ocelot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ocelot\ocelot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="136">
   <si>
     <t>parent</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>mean</t>
+  </si>
+  <si>
+    <t>Ref</t>
   </si>
 </sst>
 </file>
@@ -758,11 +761,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63:A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2030,6 +2033,74 @@
         <v>80</v>
       </c>
     </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" t="s">
+        <v>135</v>
+      </c>
+      <c r="C63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" t="s">
+        <v>18</v>
+      </c>
+      <c r="G63" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>50</v>
+      </c>
+      <c r="B66" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G62">
     <sortState ref="A2:G62">

</xml_diff>